<commit_message>
Updated models and performance improvements
Updated both the contour and bowtie models and changed input of silhouette_overlap_group to accept polygon objects for the group (instead of contours).
</commit_message>
<xml_diff>
--- a/data-raw/Indices.xlsx
+++ b/data-raw/Indices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sieli\Documents\GitHub\IQeyes\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA6FABF-CAF2-41CF-89AF-27584C88CB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC2C40-0ED5-4C35-8327-EC43E138F831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32430" yWindow="-15600" windowWidth="22515" windowHeight="14670" xr2:uid="{153E3B4F-7EDD-478F-A6A5-DF8BF2B3711C}"/>
+    <workbookView xWindow="44865" yWindow="-16425" windowWidth="29040" windowHeight="15720" xr2:uid="{153E3B4F-7EDD-478F-A6A5-DF8BF2B3711C}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="15" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="96">
   <si>
     <t>Index</t>
   </si>
@@ -162,9 +162,6 @@
     <t>PPI Ave</t>
   </si>
   <si>
-    <t>ART-max</t>
-  </si>
-  <si>
     <t xml:space="preserve">R_min </t>
   </si>
   <si>
@@ -174,12 +171,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Elev front thin</t>
-  </si>
-  <si>
-    <t>Elev back thin</t>
-  </si>
-  <si>
     <t>PI_avg</t>
   </si>
   <si>
@@ -274,6 +265,69 @@
   </si>
   <si>
     <t>pachy_prog_index_avg</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1155/2018/7875148</t>
+  </si>
+  <si>
+    <t>Topographic Asymmetry Indices: Correlation between Inferior Minus Superior Value and Index of Height Decentration</t>
+  </si>
+  <si>
+    <t>Sherine S. Wahba, Maged M. Roshdy, Ramy R. Fikry, Mona K. Abdellatif, Abdulrahman M. Abodarahim</t>
+  </si>
+  <si>
+    <t>Journal of Ophthalmology</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>Elev front thinnest</t>
+  </si>
+  <si>
+    <t>Elev back thinnest</t>
+  </si>
+  <si>
+    <t>Elevation (Front) Max. Peak</t>
+  </si>
+  <si>
+    <t>Elevation (Back) Max. Peak</t>
+  </si>
+  <si>
+    <t>ele_f_bfs_8mm_thinnest</t>
+  </si>
+  <si>
+    <t>ele_b_bfs_8mm_thinnest</t>
+  </si>
+  <si>
+    <t>art_max</t>
+  </si>
+  <si>
+    <t>bad_d</t>
+  </si>
+  <si>
+    <t>bad_dam</t>
+  </si>
+  <si>
+    <t>is_value</t>
+  </si>
+  <si>
+    <t>isv</t>
+  </si>
+  <si>
+    <t>iva</t>
+  </si>
+  <si>
+    <t>k_max</t>
+  </si>
+  <si>
+    <t>pachy_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r_min </t>
+  </si>
+  <si>
+    <t>bad_db</t>
   </si>
 </sst>
 </file>
@@ -295,15 +349,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -311,19 +371,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,7 +1275,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{29388FF0-0563-4CB4-A6B0-7F4ED1CAA250}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{29388FF0-0563-4CB4-A6B0-7F4ED1CAA250}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:P11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField axis="axisCol" showAll="0">
@@ -1333,8 +1414,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9036E7B-8081-471D-9BC8-352384F28D47}" name="Table1" displayName="Table1" ref="A1:Q46" totalsRowShown="0">
-  <autoFilter ref="A1:Q46" xr:uid="{F9036E7B-8081-471D-9BC8-352384F28D47}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9036E7B-8081-471D-9BC8-352384F28D47}" name="Table1" displayName="Table1" ref="A1:Q52" totalsRowShown="0">
+  <autoFilter ref="A1:Q52" xr:uid="{F9036E7B-8081-471D-9BC8-352384F28D47}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Normal"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{DE857924-8C9B-4215-88C1-1803EB0CD946}" name="Index"/>
     <tableColumn id="2" xr3:uid="{AF1A02C8-3577-485C-B87A-7C9526A82DEA}" name="Alias"/>
@@ -1675,15 +1762,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96DB0737-AF2F-4BE3-8388-40F7F0438F40}">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.90625" customWidth="1"/>
     <col min="7" max="8" width="12.1796875" customWidth="1"/>
     <col min="9" max="9" width="11.36328125" customWidth="1"/>
@@ -1708,51 +1795,51 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
         <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>18.3</v>
@@ -1763,9 +1850,6 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
@@ -1779,7 +1863,7 @@
         <v>24</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N2">
         <v>3</v>
@@ -1787,8 +1871,8 @@
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>66</v>
+      <c r="P2" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q2">
         <v>2014</v>
@@ -1796,10 +1880,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>1.7</v>
@@ -1810,9 +1894,6 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
@@ -1826,7 +1907,7 @@
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N3">
         <v>3</v>
@@ -1834,16 +1915,16 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>66</v>
+      <c r="P3" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q3">
         <v>2014</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="C4">
         <v>192.99</v>
@@ -1851,13 +1932,19 @@
       <c r="D4">
         <v>83.28</v>
       </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>432</v>
+      </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>14</v>
       </c>
       <c r="K4" t="s">
@@ -1867,7 +1954,7 @@
         <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1875,16 +1962,16 @@
       <c r="O4">
         <v>2</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>67</v>
+      <c r="P4" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q4">
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>209.9</v>
@@ -1905,7 +1992,7 @@
         <v>24</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N5">
         <v>3</v>
@@ -1913,19 +2000,16 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>66</v>
+      <c r="P5" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q5">
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C6">
         <v>180.78</v>
@@ -1946,7 +2030,7 @@
         <v>33</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N6">
         <v>27</v>
@@ -1954,8 +2038,8 @@
       <c r="O6">
         <v>10</v>
       </c>
-      <c r="P6" s="2" t="s">
-        <v>61</v>
+      <c r="P6" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q6">
         <v>2011</v>
@@ -1963,7 +2047,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="C7">
         <v>526.69000000000005</v>
@@ -1971,6 +2055,12 @@
       <c r="D7">
         <v>90.64</v>
       </c>
+      <c r="E7">
+        <v>219</v>
+      </c>
+      <c r="F7">
+        <v>908</v>
+      </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
@@ -1984,7 +2074,7 @@
         <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1992,8 +2082,8 @@
       <c r="O7">
         <v>2</v>
       </c>
-      <c r="P7" s="2" t="s">
-        <v>67</v>
+      <c r="P7" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q7">
         <v>2012</v>
@@ -2001,7 +2091,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="C8">
         <v>473</v>
@@ -2025,7 +2115,7 @@
         <v>24</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N8">
         <v>3</v>
@@ -2033,8 +2123,8 @@
       <c r="O8">
         <v>1</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>66</v>
+      <c r="P8" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q8">
         <v>2014</v>
@@ -2042,10 +2132,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>507.36</v>
@@ -2066,7 +2153,7 @@
         <v>33</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N9">
         <v>27</v>
@@ -2074,16 +2161,16 @@
       <c r="O9">
         <v>10</v>
       </c>
-      <c r="P9" s="2" t="s">
-        <v>61</v>
+      <c r="P9" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q9">
         <v>2011</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>8.08</v>
@@ -2091,6 +2178,12 @@
       <c r="D10">
         <v>4.99</v>
       </c>
+      <c r="E10">
+        <v>1.36</v>
+      </c>
+      <c r="F10">
+        <v>33.93</v>
+      </c>
       <c r="G10" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2197,7 @@
         <v>23</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2112,19 +2205,19 @@
       <c r="O10">
         <v>2</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>67</v>
+      <c r="P10" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q10">
         <v>2012</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>7.49</v>
@@ -2148,7 +2241,7 @@
         <v>24</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N11">
         <v>3</v>
@@ -2156,8 +2249,8 @@
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>66</v>
+      <c r="P11" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q11">
         <v>2014</v>
@@ -2165,7 +2258,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="C12">
         <v>0.43</v>
@@ -2173,6 +2266,12 @@
       <c r="D12">
         <v>0.56999999999999995</v>
       </c>
+      <c r="E12">
+        <v>-1.2</v>
+      </c>
+      <c r="F12">
+        <v>2.71</v>
+      </c>
       <c r="G12" t="s">
         <v>5</v>
       </c>
@@ -2186,7 +2285,7 @@
         <v>23</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2194,8 +2293,8 @@
       <c r="O12">
         <v>2</v>
       </c>
-      <c r="P12" s="2" t="s">
-        <v>67</v>
+      <c r="P12" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q12">
         <v>2012</v>
@@ -2203,10 +2302,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>0.69</v>
@@ -2230,7 +2329,7 @@
         <v>24</v>
       </c>
       <c r="M13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N13">
         <v>3</v>
@@ -2238,16 +2337,16 @@
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>66</v>
+      <c r="P13" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q13">
         <v>2014</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="C14">
         <v>2.7</v>
@@ -2255,6 +2354,12 @@
       <c r="D14">
         <v>0.76</v>
       </c>
+      <c r="E14">
+        <v>0.51</v>
+      </c>
+      <c r="F14">
+        <v>4.2699999999999996</v>
+      </c>
       <c r="G14" t="s">
         <v>6</v>
       </c>
@@ -2271,7 +2376,7 @@
         <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2279,8 +2384,8 @@
       <c r="O14">
         <v>2</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>67</v>
+      <c r="P14" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q14">
         <v>2012</v>
@@ -2288,7 +2393,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="C15">
         <v>-0.35</v>
@@ -2296,6 +2401,12 @@
       <c r="D15">
         <v>0.83</v>
       </c>
+      <c r="E15">
+        <v>-3.84</v>
+      </c>
+      <c r="F15">
+        <v>2.46</v>
+      </c>
       <c r="G15" t="s">
         <v>5</v>
       </c>
@@ -2312,7 +2423,7 @@
         <v>23</v>
       </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -2320,14 +2431,14 @@
       <c r="O15">
         <v>2</v>
       </c>
-      <c r="P15" s="2" t="s">
-        <v>67</v>
+      <c r="P15" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q15">
         <v>2012</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -2356,7 +2467,7 @@
         <v>33</v>
       </c>
       <c r="M16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N16">
         <v>27</v>
@@ -2364,8 +2475,8 @@
       <c r="O16">
         <v>10</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>61</v>
+      <c r="P16" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q16">
         <v>2011</v>
@@ -2400,7 +2511,7 @@
         <v>33</v>
       </c>
       <c r="M17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N17">
         <v>27</v>
@@ -2408,16 +2519,16 @@
       <c r="O17">
         <v>10</v>
       </c>
-      <c r="P17" s="2" t="s">
-        <v>61</v>
+      <c r="P17" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q17">
         <v>2011</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C18">
         <v>4.66</v>
@@ -2431,26 +2542,23 @@
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>58</v>
+      <c r="J18" t="s">
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N18">
         <v>251</v>
       </c>
-      <c r="P18" s="2" t="s">
-        <v>55</v>
+      <c r="P18" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="Q18">
         <v>2023</v>
@@ -2458,7 +2566,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>0.11</v>
@@ -2472,34 +2580,31 @@
       <c r="G19" t="s">
         <v>5</v>
       </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>58</v>
+      <c r="J19" t="s">
+        <v>55</v>
       </c>
       <c r="K19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N19">
         <v>251</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>55</v>
+      <c r="P19" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="Q19">
         <v>2023</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C20">
         <v>79.760000000000005</v>
@@ -2507,6 +2612,12 @@
       <c r="D20">
         <v>38.9</v>
       </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <v>199</v>
+      </c>
       <c r="G20" t="s">
         <v>6</v>
       </c>
@@ -2523,7 +2634,7 @@
         <v>23</v>
       </c>
       <c r="M20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -2531,16 +2642,16 @@
       <c r="O20">
         <v>2</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>67</v>
+      <c r="P20" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q20">
         <v>2012</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C21">
         <v>98.99</v>
@@ -2561,13 +2672,13 @@
         <v>26</v>
       </c>
       <c r="M21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N21">
         <v>7</v>
       </c>
-      <c r="P21" s="2" t="s">
-        <v>64</v>
+      <c r="P21" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="Q21">
         <v>2013</v>
@@ -2575,7 +2686,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C22">
         <v>20.61</v>
@@ -2583,6 +2694,12 @@
       <c r="D22">
         <v>6.39</v>
       </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>47</v>
+      </c>
       <c r="G22" t="s">
         <v>5</v>
       </c>
@@ -2599,7 +2716,7 @@
         <v>23</v>
       </c>
       <c r="M22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -2607,16 +2724,16 @@
       <c r="O22">
         <v>2</v>
       </c>
-      <c r="P22" s="2" t="s">
-        <v>67</v>
+      <c r="P22" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q22">
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C23">
         <v>0.85</v>
@@ -2624,6 +2741,12 @@
       <c r="D23">
         <v>0.45</v>
       </c>
+      <c r="E23">
+        <v>0.04</v>
+      </c>
+      <c r="F23">
+        <v>2.17</v>
+      </c>
       <c r="G23" t="s">
         <v>6</v>
       </c>
@@ -2640,7 +2763,7 @@
         <v>23</v>
       </c>
       <c r="M23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -2648,16 +2771,16 @@
       <c r="O23">
         <v>2</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>67</v>
+      <c r="P23" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q23">
         <v>2012</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C24">
         <v>1.05</v>
@@ -2675,16 +2798,16 @@
         <v>25</v>
       </c>
       <c r="L24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N24">
         <v>7</v>
       </c>
-      <c r="P24" s="2" t="s">
-        <v>64</v>
+      <c r="P24" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="Q24">
         <v>2013</v>
@@ -2692,7 +2815,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C25">
         <v>0.18</v>
@@ -2700,6 +2823,12 @@
       <c r="D25">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="E25">
+        <v>0.04</v>
+      </c>
+      <c r="F25">
+        <v>0.38</v>
+      </c>
       <c r="G25" t="s">
         <v>5</v>
       </c>
@@ -2716,7 +2845,7 @@
         <v>23</v>
       </c>
       <c r="M25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -2724,16 +2853,16 @@
       <c r="O25">
         <v>2</v>
       </c>
-      <c r="P25" s="2" t="s">
-        <v>67</v>
+      <c r="P25" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q25">
         <v>2012</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C26">
         <v>54</v>
@@ -2741,6 +2870,12 @@
       <c r="D26">
         <v>6.92</v>
       </c>
+      <c r="E26">
+        <v>43</v>
+      </c>
+      <c r="F26">
+        <v>86.1</v>
+      </c>
       <c r="G26" t="s">
         <v>6</v>
       </c>
@@ -2754,7 +2889,7 @@
         <v>23</v>
       </c>
       <c r="M26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -2762,16 +2897,16 @@
       <c r="O26">
         <v>2</v>
       </c>
-      <c r="P26" s="2" t="s">
-        <v>67</v>
+      <c r="P26" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q26">
         <v>2012</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C27">
         <v>54.9</v>
@@ -2798,7 +2933,7 @@
         <v>24</v>
       </c>
       <c r="M27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N27">
         <v>3</v>
@@ -2806,8 +2941,8 @@
       <c r="O27">
         <v>1</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>66</v>
+      <c r="P27" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q27">
         <v>2014</v>
@@ -2815,7 +2950,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C28">
         <v>44.57</v>
@@ -2823,6 +2958,12 @@
       <c r="D28">
         <v>1.5</v>
       </c>
+      <c r="E28">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F28">
+        <v>48.8</v>
+      </c>
       <c r="G28" t="s">
         <v>5</v>
       </c>
@@ -2836,7 +2977,7 @@
         <v>23</v>
       </c>
       <c r="M28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -2844,8 +2985,8 @@
       <c r="O28">
         <v>2</v>
       </c>
-      <c r="P28" s="2" t="s">
-        <v>67</v>
+      <c r="P28" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q28">
         <v>2012</v>
@@ -2853,7 +2994,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>45.3</v>
@@ -2880,7 +3021,7 @@
         <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N29">
         <v>3</v>
@@ -2888,14 +3029,14 @@
       <c r="O29">
         <v>1</v>
       </c>
-      <c r="P29" s="2" t="s">
-        <v>66</v>
+      <c r="P29" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q29">
         <v>2014</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2924,7 +3065,7 @@
         <v>33</v>
       </c>
       <c r="M30" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N30">
         <v>27</v>
@@ -2932,8 +3073,8 @@
       <c r="O30">
         <v>10</v>
       </c>
-      <c r="P30" s="2" t="s">
-        <v>61</v>
+      <c r="P30" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q30">
         <v>2011</v>
@@ -2968,7 +3109,7 @@
         <v>33</v>
       </c>
       <c r="M31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N31">
         <v>27</v>
@@ -2976,16 +3117,16 @@
       <c r="O31">
         <v>10</v>
       </c>
-      <c r="P31" s="2" t="s">
-        <v>61</v>
+      <c r="P31" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q31">
         <v>2011</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C32">
         <v>459.06</v>
@@ -2993,6 +3134,12 @@
       <c r="D32">
         <v>47.6</v>
       </c>
+      <c r="E32">
+        <v>47.6</v>
+      </c>
+      <c r="F32">
+        <v>296</v>
+      </c>
       <c r="G32" t="s">
         <v>6</v>
       </c>
@@ -3006,7 +3153,7 @@
         <v>23</v>
       </c>
       <c r="M32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N32">
         <v>1</v>
@@ -3014,19 +3161,19 @@
       <c r="O32">
         <v>2</v>
       </c>
-      <c r="P32" s="2" t="s">
-        <v>67</v>
+      <c r="P32" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q32">
         <v>2012</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>473</v>
@@ -3047,7 +3194,7 @@
         <v>24</v>
       </c>
       <c r="M33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N33">
         <v>3</v>
@@ -3055,16 +3202,16 @@
       <c r="O33">
         <v>1</v>
       </c>
-      <c r="P33" s="2" t="s">
-        <v>66</v>
+      <c r="P33" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q33">
         <v>2014</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C34">
         <v>428</v>
@@ -3085,7 +3232,7 @@
         <v>30</v>
       </c>
       <c r="M34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N34">
         <v>32</v>
@@ -3093,16 +3240,16 @@
       <c r="O34">
         <v>11</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>60</v>
+      <c r="P34" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="Q34">
         <v>2006</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
@@ -3132,7 +3279,7 @@
         <v>33</v>
       </c>
       <c r="M35" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N35">
         <v>27</v>
@@ -3140,8 +3287,8 @@
       <c r="O35">
         <v>10</v>
       </c>
-      <c r="P35" s="2" t="s">
-        <v>61</v>
+      <c r="P35" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q35">
         <v>2011</v>
@@ -3149,7 +3296,7 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C36">
         <v>549.23</v>
@@ -3157,10 +3304,16 @@
       <c r="D36">
         <v>35.47</v>
       </c>
+      <c r="E36">
+        <v>454</v>
+      </c>
+      <c r="F36">
+        <v>660</v>
+      </c>
       <c r="G36" t="s">
         <v>5</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" t="s">
         <v>14</v>
       </c>
       <c r="K36" t="s">
@@ -3170,7 +3323,7 @@
         <v>23</v>
       </c>
       <c r="M36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N36">
         <v>1</v>
@@ -3178,8 +3331,8 @@
       <c r="O36">
         <v>2</v>
       </c>
-      <c r="P36" s="2" t="s">
-        <v>67</v>
+      <c r="P36" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="Q36">
         <v>2012</v>
@@ -3187,10 +3340,10 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>539</v>
@@ -3211,7 +3364,7 @@
         <v>24</v>
       </c>
       <c r="M37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N37">
         <v>3</v>
@@ -3219,8 +3372,8 @@
       <c r="O37">
         <v>1</v>
       </c>
-      <c r="P37" s="2" t="s">
-        <v>66</v>
+      <c r="P37" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q37">
         <v>2014</v>
@@ -3228,7 +3381,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="C38">
         <v>537</v>
@@ -3249,7 +3402,7 @@
         <v>30</v>
       </c>
       <c r="M38" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="N38">
         <v>32</v>
@@ -3257,8 +3410,8 @@
       <c r="O38">
         <v>11</v>
       </c>
-      <c r="P38" s="2" t="s">
-        <v>60</v>
+      <c r="P38" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="Q38">
         <v>2006</v>
@@ -3266,7 +3419,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
@@ -3296,7 +3449,7 @@
         <v>33</v>
       </c>
       <c r="M39" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N39">
         <v>27</v>
@@ -3304,19 +3457,19 @@
       <c r="O39">
         <v>10</v>
       </c>
-      <c r="P39" s="2" t="s">
-        <v>61</v>
+      <c r="P39" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q39">
         <v>2011</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C40">
         <v>39.799999999999997</v>
@@ -3327,9 +3480,6 @@
       <c r="G40" t="s">
         <v>6</v>
       </c>
-      <c r="H40" t="b">
-        <v>1</v>
-      </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
@@ -3343,7 +3493,7 @@
         <v>24</v>
       </c>
       <c r="M40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N40">
         <v>3</v>
@@ -3351,8 +3501,8 @@
       <c r="O40">
         <v>1</v>
       </c>
-      <c r="P40" s="2" t="s">
-        <v>66</v>
+      <c r="P40" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q40">
         <v>2014</v>
@@ -3360,10 +3510,10 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="C41">
         <v>4.0999999999999996</v>
@@ -3374,9 +3524,6 @@
       <c r="G41" t="s">
         <v>5</v>
       </c>
-      <c r="H41" t="b">
-        <v>1</v>
-      </c>
       <c r="I41" t="b">
         <v>1</v>
       </c>
@@ -3390,7 +3537,7 @@
         <v>24</v>
       </c>
       <c r="M41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N41">
         <v>3</v>
@@ -3398,16 +3545,16 @@
       <c r="O41">
         <v>1</v>
       </c>
-      <c r="P41" s="2" t="s">
-        <v>66</v>
+      <c r="P41" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q41">
         <v>2014</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C42">
         <v>6.07</v>
@@ -3428,24 +3575,24 @@
         <v>26</v>
       </c>
       <c r="M42" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N42">
         <v>7</v>
       </c>
-      <c r="P42" s="2" t="s">
-        <v>64</v>
+      <c r="P42" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="Q42">
         <v>2013</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>2.09</v>
@@ -3466,7 +3613,7 @@
         <v>24</v>
       </c>
       <c r="M43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N43">
         <v>3</v>
@@ -3474,16 +3621,16 @@
       <c r="O43">
         <v>1</v>
       </c>
-      <c r="P43" s="2" t="s">
-        <v>66</v>
+      <c r="P43" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q43">
         <v>2014</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
         <v>39</v>
@@ -3513,7 +3660,7 @@
         <v>33</v>
       </c>
       <c r="M44" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N44">
         <v>27</v>
@@ -3521,8 +3668,8 @@
       <c r="O44">
         <v>10</v>
       </c>
-      <c r="P44" s="2" t="s">
-        <v>61</v>
+      <c r="P44" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q44">
         <v>2011</v>
@@ -3530,10 +3677,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C45">
         <v>0.92</v>
@@ -3554,7 +3701,7 @@
         <v>24</v>
       </c>
       <c r="M45" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N45">
         <v>3</v>
@@ -3562,8 +3709,8 @@
       <c r="O45">
         <v>1</v>
       </c>
-      <c r="P45" s="2" t="s">
-        <v>66</v>
+      <c r="P45" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="Q45">
         <v>2014</v>
@@ -3571,7 +3718,7 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
         <v>39</v>
@@ -3601,7 +3748,7 @@
         <v>33</v>
       </c>
       <c r="M46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N46">
         <v>27</v>
@@ -3609,11 +3756,203 @@
       <c r="O46">
         <v>10</v>
       </c>
-      <c r="P46" s="2" t="s">
-        <v>61</v>
+      <c r="P46" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="Q46">
         <v>2011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47">
+        <v>-0.13</v>
+      </c>
+      <c r="D47">
+        <v>0.96</v>
+      </c>
+      <c r="E47">
+        <v>-1.48</v>
+      </c>
+      <c r="F47">
+        <v>3.35</v>
+      </c>
+      <c r="G47" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>14</v>
+      </c>
+      <c r="K47" t="s">
+        <v>22</v>
+      </c>
+      <c r="L47" t="s">
+        <v>23</v>
+      </c>
+      <c r="M47" t="s">
+        <v>62</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q47">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48">
+        <v>7.05</v>
+      </c>
+      <c r="D48">
+        <v>6.21</v>
+      </c>
+      <c r="E48">
+        <v>-1.31</v>
+      </c>
+      <c r="F48">
+        <v>43.94</v>
+      </c>
+      <c r="G48" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>14</v>
+      </c>
+      <c r="K48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48" t="s">
+        <v>62</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>2</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q48">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49">
+        <v>4.62</v>
+      </c>
+      <c r="D49">
+        <v>3.89</v>
+      </c>
+      <c r="G49" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" t="s">
+        <v>75</v>
+      </c>
+      <c r="K49" t="s">
+        <v>76</v>
+      </c>
+      <c r="L49" t="s">
+        <v>77</v>
+      </c>
+      <c r="M49" t="s">
+        <v>78</v>
+      </c>
+      <c r="N49">
+        <v>2018</v>
+      </c>
+      <c r="O49">
+        <v>7875148</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q49">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50">
+        <v>0.3</v>
+      </c>
+      <c r="D50">
+        <v>0.93</v>
+      </c>
+      <c r="G50" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" t="s">
+        <v>75</v>
+      </c>
+      <c r="K50" t="s">
+        <v>76</v>
+      </c>
+      <c r="L50" t="s">
+        <v>77</v>
+      </c>
+      <c r="M50" t="s">
+        <v>78</v>
+      </c>
+      <c r="N50">
+        <v>2018</v>
+      </c>
+      <c r="O50">
+        <v>7875148</v>
+      </c>
+      <c r="P50" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q50">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3672,16 +4011,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>72</v>
+      <c r="A3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>69</v>
+      <c r="A4" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -3720,214 +4059,140 @@
         <v>19</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
         <v>18</v>
       </c>
       <c r="P4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5">
-        <v>2</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5">
+      <c r="A5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="P5">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5">
-        <v>2</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5">
-        <v>2</v>
-      </c>
-      <c r="L8" s="5">
-        <v>2</v>
-      </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5">
-        <v>2</v>
-      </c>
-      <c r="P8" s="5">
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5">
-        <v>2</v>
-      </c>
-      <c r="I9" s="5">
-        <v>2</v>
-      </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="P9">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5">
-        <v>2</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5">
-        <v>2</v>
-      </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5">
-        <v>2</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="P10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="5">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5">
-        <v>2</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2</v>
-      </c>
-      <c r="E11" s="5">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5">
-        <v>2</v>
-      </c>
-      <c r="G11" s="5">
-        <v>2</v>
-      </c>
-      <c r="H11" s="5">
-        <v>2</v>
-      </c>
-      <c r="I11" s="5">
-        <v>2</v>
-      </c>
-      <c r="J11" s="5">
-        <v>2</v>
-      </c>
-      <c r="K11" s="5">
-        <v>2</v>
-      </c>
-      <c r="L11" s="5">
-        <v>2</v>
-      </c>
-      <c r="M11" s="5">
-        <v>2</v>
-      </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5">
-        <v>2</v>
-      </c>
-      <c r="P11" s="5">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
         <v>26</v>
       </c>
     </row>

</xml_diff>